<commit_message>
chore: publish terminology IG 2.0.2
</commit_message>
<xml_diff>
--- a/ig/terminology/CodeSystem-MedComDiagnosticReportCodes.xlsx
+++ b/ig/terminology/CodeSystem-MedComDiagnosticReportCodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.1</t>
+    <t>1.8.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -45,19 +45,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-31</t>
+    <t>2025-11-18</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -334,114 +331,112 @@
       <c r="A7" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="2">
-        <v>12</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>13</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>15</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>17</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>19</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>21</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s" s="2">
         <v>25</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s" s="2">
         <v>31</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s" s="2">
         <v>34</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -459,27 +454,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>36</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="C1" t="s" s="1">
         <v>37</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="D1" t="s" s="1">
         <v>38</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s" s="2">
         <v>40</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="D2" s="2"/>
     </row>

</xml_diff>

<commit_message>
chore: publish terminology IG 2.0.2 (#54)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/terminology/CodeSystem-MedComDiagnosticReportCodes.xlsx
+++ b/ig/terminology/CodeSystem-MedComDiagnosticReportCodes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.1</t>
+    <t>1.8.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -45,19 +45,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-31</t>
+    <t>2025-11-18</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -334,114 +331,112 @@
       <c r="A7" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="2">
-        <v>12</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>13</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>15</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>17</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>19</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>21</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s" s="2">
         <v>25</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s" s="2">
         <v>31</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>32</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s" s="2">
         <v>34</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -459,27 +454,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>36</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="C1" t="s" s="1">
         <v>37</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="D1" t="s" s="1">
         <v>38</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s" s="2">
         <v>40</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>41</v>
       </c>
       <c r="D2" s="2"/>
     </row>

</xml_diff>